<commit_message>
initial commit on restel assertion
</commit_message>
<xml_diff>
--- a/Sample_Suite_definition.xlsx
+++ b/Sample_Suite_definition.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Base_Config" sheetId="1" state="visible" r:id="rId2"/>
@@ -269,10 +269,10 @@
     <t xml:space="preserve">{"body":"${val[0]}"}</t>
   </si>
   <si>
-    <t xml:space="preserve">{"Assert1": {"actual":"${fetch_pet_by_status_to_update_exec.pet_findByStatus.response[0]}","expected":"${fetch_pet_by_status_to_update_exec.pet_findByStatus.response[0]}"}, "Assert2":{"actual":"","expected":""}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{   "val": {     "operation": "remove",     "data": "${fetch_pet_by_status_to_update_exec.pet_findByStatus.response[0]}"   } }</t>
+    <t xml:space="preserve">{   "Assert1": {     "condition": [       "not_null",       "${fetch_pet_by_status_to_update_exec.pet_findByStatus.response[0].name}"    ],     "message": "Validation success"   } }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{   "val": {     "operation": "remove", "data": "${fetch_pet_by_status_to_update_exec.pet_findByStatus.response[0]}"   } }</t>
   </si>
   <si>
     <t xml:space="preserve">case_unique_name</t>
@@ -1018,8 +1018,8 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1231,7 +1231,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="179.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="128.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>60</v>
       </c>
@@ -1272,7 +1272,7 @@
   </sheetPr>
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
     </sheetView>
   </sheetViews>

</xml_diff>